<commit_message>
adding CS topic for intro CS courses
</commit_message>
<xml_diff>
--- a/data/cs-courses_2019-2020.xlsx
+++ b/data/cs-courses_2019-2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kapilgarg/Documents/Northwestern/phd/conversational-interfaces/CI_TeachingKiosk/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BF4777-4F43-8D45-9233-6610240D2981}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AC7A5C-8233-E34B-804B-7A275FDC9622}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="64000" yWindow="-4340" windowWidth="25600" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="-11540" windowWidth="32000" windowHeight="35540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="By course" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="182">
   <si>
     <t>Course</t>
   </si>
@@ -577,6 +577,9 @@
   </si>
   <si>
     <t>SoftwareSystemStructures-Topic</t>
+  </si>
+  <si>
+    <t>ComputerScience</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +1008,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1071,6 +1074,9 @@
       <c r="E2" s="7" t="s">
         <v>30</v>
       </c>
+      <c r="F2" s="7" t="s">
+        <v>181</v>
+      </c>
       <c r="G2" s="7" t="s">
         <v>7</v>
       </c>
@@ -1099,6 +1105,9 @@
       <c r="E3" s="7" t="s">
         <v>92</v>
       </c>
+      <c r="F3" s="7" t="s">
+        <v>181</v>
+      </c>
       <c r="G3" s="7" t="s">
         <v>7</v>
       </c>
@@ -1130,6 +1139,9 @@
       <c r="E4" s="7" t="s">
         <v>92</v>
       </c>
+      <c r="F4" s="7" t="s">
+        <v>181</v>
+      </c>
       <c r="G4" s="7" t="s">
         <v>7</v>
       </c>
@@ -1162,6 +1174,9 @@
       <c r="E5" s="7" t="s">
         <v>92</v>
       </c>
+      <c r="F5" s="7" t="s">
+        <v>181</v>
+      </c>
       <c r="G5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1194,6 +1209,9 @@
       <c r="E6" s="7" t="s">
         <v>104</v>
       </c>
+      <c r="F6" s="7" t="s">
+        <v>181</v>
+      </c>
       <c r="G6" s="7" t="s">
         <v>7</v>
       </c>
@@ -1226,6 +1244,9 @@
       <c r="E7" s="7" t="s">
         <v>18</v>
       </c>
+      <c r="F7" s="7" t="s">
+        <v>181</v>
+      </c>
       <c r="G7" s="7" t="s">
         <v>12</v>
       </c>
@@ -1258,6 +1279,9 @@
       <c r="E8" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="F8" s="7" t="s">
+        <v>181</v>
+      </c>
       <c r="G8" s="7" t="s">
         <v>7</v>
       </c>
@@ -1322,6 +1346,9 @@
       <c r="E10" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="F10" s="7" t="s">
+        <v>181</v>
+      </c>
       <c r="G10" s="7" t="s">
         <v>12</v>
       </c>
@@ -1354,6 +1381,9 @@
       <c r="E11" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="F11" s="7" t="s">
+        <v>181</v>
+      </c>
       <c r="G11" s="7" t="s">
         <v>12</v>
       </c>
@@ -1386,6 +1416,9 @@
       <c r="E12" s="7" t="s">
         <v>18</v>
       </c>
+      <c r="F12" s="7" t="s">
+        <v>181</v>
+      </c>
       <c r="G12" s="7" t="s">
         <v>12</v>
       </c>
@@ -1834,6 +1867,9 @@
       <c r="E25" s="7" t="s">
         <v>18</v>
       </c>
+      <c r="F25" s="7" t="s">
+        <v>181</v>
+      </c>
       <c r="G25" s="7" t="s">
         <v>12</v>
       </c>
@@ -1897,6 +1933,9 @@
       </c>
       <c r="E27" s="7" t="s">
         <v>17</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>181</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>7</v>

</xml_diff>